<commit_message>
Improved experiment values for CI, saved results
</commit_message>
<xml_diff>
--- a/results_final/ci_HH.xlsx
+++ b/results_final/ci_HH.xlsx
@@ -519,91 +519,91 @@
         <v>0.236257522822892</v>
       </c>
       <c r="D2">
-        <v>0.2353808692170102</v>
+        <v>0.2353989116639682</v>
       </c>
       <c r="E2">
-        <v>0.2345336233158151</v>
+        <v>0.234586121489699</v>
       </c>
       <c r="F2">
-        <v>0.2337147086699072</v>
+        <v>0.2338165704190317</v>
       </c>
       <c r="G2">
-        <v>0.2329230935552905</v>
+        <v>0.2330878353329215</v>
       </c>
       <c r="H2">
-        <v>0.2321577888095908</v>
+        <v>0.2323976408515991</v>
       </c>
       <c r="I2">
-        <v>0.2314178457898681</v>
+        <v>0.2317438491920368</v>
       </c>
       <c r="J2">
-        <v>0.2307023544442605</v>
+        <v>0.2311244508253069</v>
       </c>
       <c r="K2">
-        <v>0.2300104414902487</v>
+        <v>0.2305375558617144</v>
       </c>
       <c r="L2">
-        <v>0.2293412686928342</v>
+        <v>0.22998138609886</v>
       </c>
       <c r="M2">
-        <v>0.2286940312363973</v>
+        <v>0.2294542676742649</v>
       </c>
       <c r="N2">
-        <v>0.2280679561844266</v>
+        <v>0.2289546242699487</v>
       </c>
       <c r="O2">
-        <v>0.2274623010217193</v>
+        <v>0.2284809708214959</v>
       </c>
       <c r="P2">
-        <v>0.2268763522740143</v>
+        <v>0.2280319076887334</v>
       </c>
       <c r="Q2">
-        <v>0.2263094242003667</v>
+        <v>0.2276061152492428</v>
       </c>
       <c r="R2">
-        <v>0.2257608575538867</v>
+        <v>0.2272023488796025</v>
       </c>
       <c r="S2">
-        <v>0.2252300184067607</v>
+        <v>0.2268194342925423</v>
       </c>
       <c r="T2">
-        <v>0.2247162970357427</v>
+        <v>0.226456263201139</v>
       </c>
       <c r="U2">
-        <v>0.2242191068645566</v>
+        <v>0.2261117892838335</v>
       </c>
       <c r="V2">
-        <v>0.2237378834598853</v>
+        <v>0.2257850244264218</v>
       </c>
       <c r="W2">
-        <v>0.223272083577837</v>
+        <v>0.22547503521932</v>
       </c>
       <c r="X2">
-        <v>0.222821184257982</v>
+        <v>0.2251809396903237</v>
       </c>
       <c r="Y2">
-        <v>0.2223846819622407</v>
+        <v>0.2249019042548259</v>
       </c>
       <c r="Z2">
-        <v>0.2219620917560774</v>
+        <v>0.2246371408670206</v>
       </c>
       <c r="AA2">
-        <v>0.2215529465296144</v>
+        <v>0.2243859043570396</v>
       </c>
       <c r="AB2">
-        <v>0.221156796256435</v>
+        <v>0.2241474899402487</v>
       </c>
       <c r="AC2">
-        <v>0.2207732072879802</v>
+        <v>0.2239212308860907</v>
       </c>
       <c r="AD2">
-        <v>0.2204017616815782</v>
+        <v>0.2237064963349106</v>
       </c>
       <c r="AE2">
-        <v>0.2200420565602632</v>
+        <v>0.2235026892521549</v>
       </c>
       <c r="AF2">
-        <v>0.2196937035026567</v>
+        <v>0.2233092445101985</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -611,97 +611,97 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.2141411028578384</v>
+        <v>0.2141411028578385</v>
       </c>
       <c r="C3">
-        <v>0.2093131140741206</v>
+        <v>0.2093131140741207</v>
       </c>
       <c r="D3">
-        <v>0.2047339902384919</v>
+        <v>0.2048273860912341</v>
       </c>
       <c r="E3">
-        <v>0.2003879753606218</v>
+        <v>0.2006550190546941</v>
       </c>
       <c r="F3">
-        <v>0.1962605053014516</v>
+        <v>0.1967700208887521</v>
       </c>
       <c r="G3">
-        <v>0.1923381038670194</v>
+        <v>0.1931489674780663</v>
       </c>
       <c r="H3">
-        <v>0.1886082890589852</v>
+        <v>0.1897707076413269</v>
       </c>
       <c r="I3">
-        <v>0.1850594883890696</v>
+        <v>0.1866161063809285</v>
       </c>
       <c r="J3">
-        <v>0.1816809622923576</v>
+        <v>0.1836678209237655</v>
       </c>
       <c r="K3">
-        <v>0.1784627347861001</v>
+        <v>0.1809101049236189</v>
       </c>
       <c r="L3">
-        <v>0.1753955306184124</v>
+        <v>0.1783286369073486</v>
       </c>
       <c r="M3">
-        <v>0.172470718236983</v>
+        <v>0.1759103696409452</v>
       </c>
       <c r="N3">
-        <v>0.1696802579831504</v>
+        <v>0.1736433975883158</v>
       </c>
       <c r="O3">
-        <v>0.1670166549828405</v>
+        <v>0.1715168400524137</v>
       </c>
       <c r="P3">
-        <v>0.1644729162640756</v>
+        <v>0.1695207379387807</v>
       </c>
       <c r="Q3">
-        <v>0.1620425116820592</v>
+        <v>0.1676459623770289</v>
       </c>
       <c r="R3">
-        <v>0.1597193382781166</v>
+        <v>0.1658841336854859</v>
       </c>
       <c r="S3">
-        <v>0.1574976877387534</v>
+        <v>0.1642275493757507</v>
       </c>
       <c r="T3">
-        <v>0.1553722166564783</v>
+        <v>0.1626691200735127</v>
       </c>
       <c r="U3">
-        <v>0.1533379193253548</v>
+        <v>0.1612023123848256</v>
       </c>
       <c r="V3">
-        <v>0.1513901028320307</v>
+        <v>0.1598210978673882</v>
       </c>
       <c r="W3">
-        <v>0.1495243642276441</v>
+        <v>0.1585199073778035</v>
       </c>
       <c r="X3">
-        <v>0.1477365695879189</v>
+        <v>0.1572935901612176</v>
       </c>
       <c r="Y3">
-        <v>0.1460228347882546</v>
+        <v>0.156137377131649</v>
       </c>
       <c r="Z3">
-        <v>0.1443795078379783</v>
+        <v>0.155046847861757</v>
       </c>
       <c r="AA3">
-        <v>0.1428031526334052</v>
+        <v>0.1540179008614916</v>
       </c>
       <c r="AB3">
-        <v>0.1412905340031709</v>
+        <v>0.1530467267774693</v>
       </c>
       <c r="AC3">
-        <v>0.1398386039316455</v>
+        <v>0.1521297841902373</v>
       </c>
       <c r="AD3">
-        <v>0.1384444888572793</v>
+        <v>0.1512637777258588</v>
       </c>
       <c r="AE3">
-        <v>0.1371054779526161</v>
+        <v>0.1504456382323428</v>
       </c>
       <c r="AF3">
-        <v>0.1358190123015722</v>
+        <v>0.1496725048010793</v>
       </c>
     </row>
     <row r="4" spans="1:32">
@@ -715,91 +715,91 @@
         <v>0.2083631273380663</v>
       </c>
       <c r="D4">
-        <v>0.2044778521413778</v>
+        <v>0.2045572247431655</v>
       </c>
       <c r="E4">
-        <v>0.2007783680226081</v>
+        <v>0.2010060276077023</v>
       </c>
       <c r="F4">
-        <v>0.1972538305636888</v>
+        <v>0.197689510457897</v>
       </c>
       <c r="G4">
-        <v>0.1938941543279754</v>
+        <v>0.1945895186528332</v>
       </c>
       <c r="H4">
-        <v>0.1906899512951862</v>
+        <v>0.1916895644949511</v>
       </c>
       <c r="I4">
-        <v>0.187632474919315</v>
+        <v>0.1889746485295334</v>
       </c>
       <c r="J4">
-        <v>0.1847135692425109</v>
+        <v>0.1864311025869847</v>
       </c>
       <c r="K4">
-        <v>0.1819256225601941</v>
+        <v>0.1840464516357482</v>
       </c>
       <c r="L4">
-        <v>0.179261525187569</v>
+        <v>0.1818092919450447</v>
       </c>
       <c r="M4">
-        <v>0.1767146309261649</v>
+        <v>0.1797091834194964</v>
       </c>
       <c r="N4">
-        <v>0.1742787218718523</v>
+        <v>0.1777365542737401</v>
       </c>
       <c r="O4">
-        <v>0.171947976243691</v>
+        <v>0.1758826164738587</v>
       </c>
       <c r="P4">
-        <v>0.1697169389465298</v>
+        <v>0.1741392905917176</v>
       </c>
       <c r="Q4">
-        <v>0.1675804946100619</v>
+        <v>0.1724991389045137</v>
       </c>
       <c r="R4">
-        <v>0.1655338428734791</v>
+        <v>0.1709553057303786</v>
       </c>
       <c r="S4">
-        <v>0.1635724757083744</v>
+        <v>0.1695014641261295</v>
       </c>
       <c r="T4">
-        <v>0.1616921565934607</v>
+        <v>0.1681317681888997</v>
       </c>
       <c r="U4">
-        <v>0.1598889013733139</v>
+        <v>0.1668408103024582</v>
       </c>
       <c r="V4">
-        <v>0.1581589606499675</v>
+        <v>0.1656235827540845</v>
       </c>
       <c r="W4">
-        <v>0.1564988035710308</v>
+        <v>0.1644754432210419</v>
       </c>
       <c r="X4">
-        <v>0.154905102891267</v>
+        <v>0.1633920836887537</v>
       </c>
       <c r="Y4">
-        <v>0.1533747211964339</v>
+        <v>0.162369502417254</v>
       </c>
       <c r="Z4">
-        <v>0.1519046981888214</v>
+        <v>0.1614039786195993</v>
       </c>
       <c r="AA4">
-        <v>0.1504922389434471</v>
+        <v>0.160492049556768</v>
       </c>
       <c r="AB4">
-        <v>0.1491347030524241</v>
+        <v>0.1596304897890296</v>
       </c>
       <c r="AC4">
-        <v>0.1478295945826932</v>
+        <v>0.15881629235461</v>
       </c>
       <c r="AD4">
-        <v>0.1465745527792195</v>
+        <v>0.1580466516733422</v>
       </c>
       <c r="AE4">
-        <v>0.1453673434519687</v>
+        <v>0.1573189479964449</v>
       </c>
       <c r="AF4">
-        <v>0.144205850990573</v>
+        <v>0.1566307332440598</v>
       </c>
     </row>
     <row r="5" spans="1:32">
@@ -813,91 +813,91 @@
         <v>0.2340017226395489</v>
       </c>
       <c r="D5">
-        <v>0.232755967266229</v>
+        <v>0.232781585860701</v>
       </c>
       <c r="E5">
-        <v>0.2315539214649986</v>
+        <v>0.2316283492946909</v>
       </c>
       <c r="F5">
-        <v>0.2303938686347166</v>
+        <v>0.2305380669527254</v>
       </c>
       <c r="G5">
-        <v>0.2292741704593106</v>
+        <v>0.2295070526118231</v>
       </c>
       <c r="H5">
-        <v>0.2281932627116679</v>
+        <v>0.2285318601632405</v>
       </c>
       <c r="I5">
-        <v>0.2271496513177404</v>
+        <v>0.2276092656787824</v>
       </c>
       <c r="J5">
-        <v>0.2261419086626763</v>
+        <v>0.2267362510244439</v>
       </c>
       <c r="K5">
-        <v>0.2251686701221905</v>
+        <v>0.2259099888696062</v>
       </c>
       <c r="L5">
-        <v>0.2242286308036737</v>
+        <v>0.2251278289565359</v>
       </c>
       <c r="M5">
-        <v>0.2233205424827177</v>
+        <v>0.2243872855095</v>
       </c>
       <c r="N5">
-        <v>0.2224432107218144</v>
+        <v>0.2236860256756687</v>
       </c>
       <c r="O5">
-        <v>0.2215954921589786</v>
+        <v>0.2230218589013362</v>
       </c>
       <c r="P5">
-        <v>0.2207762919549557</v>
+        <v>0.2223927271570489</v>
       </c>
       <c r="Q5">
-        <v>0.2199845613885103</v>
+        <v>0.2217966959341401</v>
       </c>
       <c r="R5">
-        <v>0.2192192955900661</v>
+        <v>0.2212319459430772</v>
       </c>
       <c r="S5">
-        <v>0.2184795314046698</v>
+        <v>0.220696765451051</v>
       </c>
       <c r="T5">
-        <v>0.217764345375908</v>
+        <v>0.2201895432024899</v>
       </c>
       <c r="U5">
-        <v>0.2170728518430058</v>
+        <v>0.2197087618717394</v>
       </c>
       <c r="V5">
-        <v>0.2164042011438882</v>
+        <v>0.2192529920021172</v>
       </c>
       <c r="W5">
-        <v>0.215757577917497</v>
+        <v>0.2188208863899781</v>
       </c>
       <c r="X5">
-        <v>0.2151321994991278</v>
+        <v>0.2184111748763849</v>
       </c>
       <c r="Y5">
-        <v>0.2145273144029842</v>
+        <v>0.2180226595125231</v>
       </c>
       <c r="Z5">
-        <v>0.2139422008865519</v>
+        <v>0.2176542100681705</v>
       </c>
       <c r="AA5">
-        <v>0.2133761655917637</v>
+        <v>0.2173047598553771</v>
       </c>
       <c r="AB5">
-        <v>0.2128285422582712</v>
+        <v>0.2169733018420666</v>
       </c>
       <c r="AC5">
-        <v>0.2122986905044585</v>
+        <v>0.2166588850325647</v>
       </c>
       <c r="AD5">
-        <v>0.2117859946721234</v>
+        <v>0.2163606110941255</v>
       </c>
       <c r="AE5">
-        <v>0.21128986273103</v>
+        <v>0.2160776312103875</v>
       </c>
       <c r="AF5">
-        <v>0.2108097252397839</v>
+        <v>0.2158091431443639</v>
       </c>
     </row>
     <row r="6" spans="1:32">
@@ -905,97 +905,97 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.2578654048909472</v>
+        <v>0.2578654048909471</v>
       </c>
       <c r="C6">
         <v>0.254309962413845</v>
       </c>
       <c r="D6">
-        <v>0.250908028107891</v>
+        <v>0.2509777094958207</v>
       </c>
       <c r="E6">
-        <v>0.2476516383586561</v>
+        <v>0.2478525208440144</v>
       </c>
       <c r="F6">
-        <v>0.2445333255463132</v>
+        <v>0.2449196441728598</v>
       </c>
       <c r="G6">
-        <v>0.2415460819582486</v>
+        <v>0.242165563364851</v>
       </c>
       <c r="H6">
-        <v>0.2386833266780123</v>
+        <v>0.2395778771942504</v>
       </c>
       <c r="I6">
-        <v>0.2359388751783504</v>
+        <v>0.2371451916440113</v>
       </c>
       <c r="J6">
-        <v>0.2333069113732834</v>
+        <v>0.2348570241188025</v>
       </c>
       <c r="K6">
-        <v>0.230781961908468</v>
+        <v>0.2327037180888544</v>
       </c>
       <c r="L6">
-        <v>0.2283588724907604</v>
+        <v>0.2306763668969279</v>
       </c>
       <c r="M6">
-        <v>0.2260327860772671</v>
+        <v>0.228766745629466</v>
       </c>
       <c r="N6">
-        <v>0.2237991227615046</v>
+        <v>0.2269672500974408</v>
       </c>
       <c r="O6">
-        <v>0.2216535612098111</v>
+        <v>0.2252708420962953</v>
       </c>
       <c r="P6">
-        <v>0.2195920215150698</v>
+        <v>0.2236710002208649</v>
       </c>
       <c r="Q6">
-        <v>0.2176106493472897</v>
+        <v>0.2221616756028469</v>
       </c>
       <c r="R6">
-        <v>0.2157058012918094</v>
+        <v>0.2207372520175029</v>
       </c>
       <c r="S6">
-        <v>0.2138740312759712</v>
+        <v>0.2193925098746541</v>
       </c>
       <c r="T6">
-        <v>0.2121120779941892</v>
+        <v>0.2181225936682523</v>
       </c>
       <c r="U6">
-        <v>0.2104168532495133</v>
+        <v>0.2169229825101804</v>
       </c>
       <c r="V6">
-        <v>0.2087854311371543</v>
+        <v>0.2157894634185825</v>
       </c>
       <c r="W6">
-        <v>0.207215038002095</v>
+        <v>0.2147181070698894</v>
       </c>
       <c r="X6">
-        <v>0.2057030431089109</v>
+        <v>0.2137052457575987</v>
       </c>
       <c r="Y6">
-        <v>0.2042469499673601</v>
+        <v>0.2127474533304647</v>
       </c>
       <c r="Z6">
-        <v>0.2028443882622111</v>
+        <v>0.2118415269086514</v>
       </c>
       <c r="AA6">
-        <v>0.201493106340228</v>
+        <v>0.2109844701990903</v>
       </c>
       <c r="AB6">
-        <v>0.2001909642112622</v>
+        <v>0.210173478251189</v>
       </c>
       <c r="AC6">
-        <v>0.1989359270240586</v>
+        <v>0.2094059235115381</v>
       </c>
       <c r="AD6">
-        <v>0.1977260589806993</v>
+        <v>0.2086793430516577</v>
       </c>
       <c r="AE6">
-        <v>0.1965595176566291</v>
+        <v>0.207991426856398</v>
       </c>
       <c r="AF6">
-        <v>0.1954345486959423</v>
+        <v>0.2073400070725841</v>
       </c>
     </row>
     <row r="7" spans="1:32">
@@ -1009,91 +1009,91 @@
         <v>0.2827013628419978</v>
       </c>
       <c r="D7">
-        <v>0.2367126764642934</v>
+        <v>0.2375807988773385</v>
       </c>
       <c r="E7">
-        <v>0.1992637601689073</v>
+        <v>0.2014051645179322</v>
       </c>
       <c r="F7">
-        <v>0.1686082894939804</v>
+        <v>0.1721539151322304</v>
       </c>
       <c r="G7">
-        <v>0.1433857544386656</v>
+        <v>0.1483101554182984</v>
       </c>
       <c r="H7">
-        <v>0.1225305199598744</v>
+        <v>0.1287247855009627</v>
       </c>
       <c r="I7">
-        <v>0.1052035509885108</v>
+        <v>0.1125197864587716</v>
       </c>
       <c r="J7">
-        <v>0.09074086980595773</v>
+        <v>0.09901871490563889</v>
       </c>
       <c r="K7">
-        <v>0.07861443557027049</v>
+        <v>0.08769629641539024</v>
       </c>
       <c r="L7">
-        <v>0.0684022964659543</v>
+        <v>0.07814154996018467</v>
       </c>
       <c r="M7">
-        <v>0.0597657003299742</v>
+        <v>0.07003058456991793</v>
       </c>
       <c r="N7">
-        <v>0.0524314542279633</v>
+        <v>0.06310636939891738</v>
       </c>
       <c r="O7">
-        <v>0.04617826345644724</v>
+        <v>0.05716357304863166</v>
       </c>
       <c r="P7">
-        <v>0.04082610235999205</v>
+        <v>0.0520371172836641</v>
       </c>
       <c r="Q7">
-        <v>0.03622790609651104</v>
+        <v>0.0475934732468092</v>
       </c>
       <c r="R7">
-        <v>0.03226304747778826</v>
+        <v>0.04372399751558433</v>
       </c>
       <c r="S7">
-        <v>0.02883219300378817</v>
+        <v>0.04033979614643945</v>
       </c>
       <c r="T7">
-        <v>0.0258532292390701</v>
+        <v>0.03736774112171873</v>
       </c>
       <c r="U7">
-        <v>0.02325802344795883</v>
+        <v>0.0347473616642687</v>
       </c>
       <c r="V7">
-        <v>0.0209898372301642</v>
+        <v>0.03242840394449725</v>
       </c>
       <c r="W7">
-        <v>0.01900125339082535</v>
+        <v>0.03036890456353438</v>
       </c>
       <c r="X7">
-        <v>0.01725250781895381</v>
+        <v>0.02853366129734416</v>
       </c>
       <c r="Y7">
-        <v>0.01571014222608528</v>
+        <v>0.02689301276227064</v>
       </c>
       <c r="Z7">
-        <v>0.01434591205523554</v>
+        <v>0.02542185962938583</v>
       </c>
       <c r="AA7">
-        <v>0.01313589807853249</v>
+        <v>0.02409887571246036</v>
       </c>
       <c r="AB7">
-        <v>0.01205978118251046</v>
+        <v>0.0229058690758954</v>
       </c>
       <c r="AC7">
-        <v>0.01110024835942141</v>
+        <v>0.02182726226225928</v>
       </c>
       <c r="AD7">
-        <v>0.01024250455798088</v>
+        <v>0.02084966755743948</v>
       </c>
       <c r="AE7">
-        <v>0.009473870233796859</v>
+        <v>0.01996153843163399</v>
       </c>
       <c r="AF7">
-        <v>0.008783448509238748</v>
+        <v>0.01915288231170591</v>
       </c>
     </row>
     <row r="8" spans="1:32">
@@ -1107,91 +1107,91 @@
         <v>0.3848931328742282</v>
       </c>
       <c r="D8">
-        <v>0.3364687667974589</v>
+        <v>0.3374028800724147</v>
       </c>
       <c r="E8">
-        <v>0.2953256798368299</v>
+        <v>0.2977261469810976</v>
       </c>
       <c r="F8">
-        <v>0.2602297680729619</v>
+        <v>0.2643636619690402</v>
       </c>
       <c r="G8">
-        <v>0.2301765434940095</v>
+        <v>0.2361387728742781</v>
       </c>
       <c r="H8">
-        <v>0.2043450071227889</v>
+        <v>0.2121214405622078</v>
       </c>
       <c r="I8">
-        <v>0.1820614128020484</v>
+        <v>0.1915715311371804</v>
       </c>
       <c r="J8">
-        <v>0.1627706770491966</v>
+        <v>0.1738961843391066</v>
       </c>
       <c r="K8">
-        <v>0.1460137260030363</v>
+        <v>0.1586175293674642</v>
       </c>
       <c r="L8">
-        <v>0.1314094724056506</v>
+        <v>0.1453480644718466</v>
       </c>
       <c r="M8">
-        <v>0.1186404185495185</v>
+        <v>0.133771753875163</v>
       </c>
       <c r="N8">
-        <v>0.1074411105516951</v>
+        <v>0.1236294197683007</v>
       </c>
       <c r="O8">
-        <v>0.09758884381209118</v>
+        <v>0.1147073826543392</v>
       </c>
       <c r="P8">
-        <v>0.08889615279424211</v>
+        <v>0.1068285743575315</v>
       </c>
       <c r="Q8">
-        <v>0.08120472049454054</v>
+        <v>0.0998455450205171</v>
       </c>
       <c r="R8">
-        <v>0.07438042169545432</v>
+        <v>0.09363492959713308</v>
       </c>
       <c r="S8">
-        <v>0.06830927497305291</v>
+        <v>0.08809304557277355</v>
       </c>
       <c r="T8">
-        <v>0.06289412568201477</v>
+        <v>0.08313237240550678</v>
       </c>
       <c r="U8">
-        <v>0.05805191896016696</v>
+        <v>0.07867872194189282</v>
       </c>
       <c r="V8">
-        <v>0.05371145059032339</v>
+        <v>0.07466895316364369</v>
       </c>
       <c r="W8">
-        <v>0.04981150616005595</v>
+        <v>0.07104911791381303</v>
       </c>
       <c r="X8">
-        <v>0.0462993167650434</v>
+        <v>0.06777294952475092</v>
       </c>
       <c r="Y8">
-        <v>0.04312927357603332</v>
+        <v>0.06480062556041083</v>
       </c>
       <c r="Z8">
-        <v>0.04026185475274034</v>
+        <v>0.06209775068669787</v>
       </c>
       <c r="AA8">
-        <v>0.03766272707177584</v>
+        <v>0.05963451709803407</v>
       </c>
       <c r="AB8">
-        <v>0.0353019917284383</v>
+        <v>0.05738500877455303</v>
       </c>
       <c r="AC8">
-        <v>0.03315354945300424</v>
+        <v>0.05532662273299117</v>
       </c>
       <c r="AD8">
-        <v>0.03119456464628144</v>
+        <v>0.05343958582350226</v>
       </c>
       <c r="AE8">
-        <v>0.02940501191730281</v>
+        <v>0.05170654985966</v>
       </c>
       <c r="AF8">
-        <v>0.0277672913789817</v>
+        <v>0.05011225121151869</v>
       </c>
     </row>
     <row r="9" spans="1:32">
@@ -1199,97 +1199,97 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.2300599835057191</v>
+        <v>0.230059983505719</v>
       </c>
       <c r="C9">
-        <v>0.2258272331623234</v>
+        <v>0.2258272331623233</v>
       </c>
       <c r="D9">
-        <v>0.2217958858089483</v>
+        <v>0.2218782753050053</v>
       </c>
       <c r="E9">
-        <v>0.2179542506095806</v>
+        <v>0.2181907453123839</v>
       </c>
       <c r="F9">
-        <v>0.2142914505790406</v>
+        <v>0.2147443731245232</v>
       </c>
       <c r="G9">
-        <v>0.2107973568947448</v>
+        <v>0.2115207544317164</v>
       </c>
       <c r="H9">
-        <v>0.2074625291800313</v>
+        <v>0.2085031501929827</v>
       </c>
       <c r="I9">
-        <v>0.2042781611595758</v>
+        <v>0.2056763106003756</v>
       </c>
       <c r="J9">
-        <v>0.2012360311529839</v>
+        <v>0.2030263201856793</v>
       </c>
       <c r="K9">
-        <v>0.1983284569304672</v>
+        <v>0.2005404612529879</v>
       </c>
       <c r="L9">
-        <v>0.1955482545055843</v>
+        <v>0.1982070932301413</v>
       </c>
       <c r="M9">
-        <v>0.1928887004851866</v>
+        <v>0.1960155458772167</v>
       </c>
       <c r="N9">
-        <v>0.1903434976366916</v>
+        <v>0.1939560245820292</v>
       </c>
       <c r="O9">
-        <v>0.187906743368245</v>
+        <v>0.1920195262197518</v>
       </c>
       <c r="P9">
-        <v>0.18557290084878</v>
+        <v>0.1901977642636246</v>
       </c>
       <c r="Q9">
-        <v>0.1833367725229224</v>
+        <v>0.1884831020123163</v>
       </c>
       <c r="R9">
-        <v>0.1811934758005402</v>
+        <v>0.1868684929518215</v>
       </c>
       <c r="S9">
-        <v>0.1791384207228601</v>
+        <v>0.185347427399973</v>
       </c>
       <c r="T9">
-        <v>0.1771672894267969</v>
+        <v>0.1839138846931571</v>
       </c>
       <c r="U9">
-        <v>0.1752760172467398</v>
+        <v>0.1825622902705355</v>
       </c>
       <c r="V9">
-        <v>0.1734607753087595</v>
+        <v>0.1812874770933813</v>
       </c>
       <c r="W9">
-        <v>0.1717179544862561</v>
+        <v>0.1800846509080651</v>
       </c>
       <c r="X9">
-        <v>0.1700441505986495</v>
+        <v>0.1789493589224566</v>
       </c>
       <c r="Y9">
-        <v>0.1684361507459889</v>
+        <v>0.1778774615184664</v>
       </c>
       <c r="Z9">
-        <v>0.1668909206824666</v>
+        <v>0.1768651066693434</v>
       </c>
       <c r="AA9">
-        <v>0.1654055931409</v>
+        <v>0.1759087067701765</v>
       </c>
       <c r="AB9">
-        <v>0.1639774570284013</v>
+        <v>0.1750049176246876</v>
       </c>
       <c r="AC9">
-        <v>0.162603947420793</v>
+        <v>0.174150619361573</v>
       </c>
       <c r="AD9">
-        <v>0.1612826362899307</v>
+        <v>0.1733428990799721</v>
       </c>
       <c r="AE9">
-        <v>0.1600112239040477</v>
+        <v>0.1725790350466443</v>
       </c>
       <c r="AF9">
-        <v>0.1587875308466054</v>
+        <v>0.1718564822875689</v>
       </c>
     </row>
     <row r="10" spans="1:32">
@@ -1297,97 +1297,97 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.8090798252082535</v>
+        <v>0.8090798252082542</v>
       </c>
       <c r="C10">
-        <v>0.8352602500361936</v>
+        <v>0.8352602500361945</v>
       </c>
       <c r="D10">
-        <v>0.8614644149822863</v>
+        <v>0.8609159097355898</v>
       </c>
       <c r="E10">
-        <v>0.8876676754575019</v>
+        <v>0.8860183315857989</v>
       </c>
       <c r="F10">
-        <v>0.9138461282369713</v>
+        <v>0.9105432570454427</v>
       </c>
       <c r="G10">
-        <v>0.9399766533093427</v>
+        <v>0.9344704314036761</v>
       </c>
       <c r="H10">
-        <v>0.9660369497609728</v>
+        <v>0.9577833791041955</v>
       </c>
       <c r="I10">
-        <v>0.9920055659250134</v>
+        <v>0.9804691693561933</v>
       </c>
       <c r="J10">
-        <v>1.017861924047406</v>
+        <v>1.002518176102499</v>
       </c>
       <c r="K10">
-        <v>1.043586339739301</v>
+        <v>1.023923835887713</v>
       </c>
       <c r="L10">
-        <v>1.069160036498788</v>
+        <v>1.044682406666688</v>
       </c>
       <c r="M10">
-        <v>1.094565155594367</v>
+        <v>1.064792730122391</v>
       </c>
       <c r="N10">
-        <v>1.119784761608706</v>
+        <v>1.084255999625942</v>
       </c>
       <c r="O10">
-        <v>1.144802843944167</v>
+        <v>1.103075535572994</v>
       </c>
       <c r="P10">
-        <v>1.169604314591721</v>
+        <v>1.121256569470496</v>
       </c>
       <c r="Q10">
-        <v>1.194175002462573</v>
+        <v>1.138806037826197</v>
       </c>
       <c r="R10">
-        <v>1.218501644577259</v>
+        <v>1.155732386609058</v>
       </c>
       <c r="S10">
-        <v>1.242571874400598</v>
+        <v>1.172045386800429</v>
       </c>
       <c r="T10">
-        <v>1.266374207602887</v>
+        <v>1.187755961341344</v>
       </c>
       <c r="U10">
-        <v>1.289898025518352</v>
+        <v>1.202876023598204</v>
       </c>
       <c r="V10">
-        <v>1.313133556561428</v>
+        <v>1.217418327314953</v>
       </c>
       <c r="W10">
-        <v>1.336071855850105</v>
+        <v>1.231396327891881</v>
       </c>
       <c r="X10">
-        <v>1.358704783273553</v>
+        <v>1.244824054726831</v>
       </c>
       <c r="Y10">
-        <v>1.38102498022873</v>
+        <v>1.25771599427123</v>
       </c>
       <c r="Z10">
-        <v>1.403025845237868</v>
+        <v>1.270086983388566</v>
       </c>
       <c r="AA10">
-        <v>1.424701508645672</v>
+        <v>1.281952112554266</v>
       </c>
       <c r="AB10">
-        <v>1.446046806582067</v>
+        <v>1.293326638401383</v>
       </c>
       <c r="AC10">
-        <v>1.467057254363272</v>
+        <v>1.304225905093833</v>
       </c>
       <c r="AD10">
-        <v>1.487729019491229</v>
+        <v>1.314665273996567</v>
       </c>
       <c r="AE10">
-        <v>1.508058894398777</v>
+        <v>1.324660061108146</v>
       </c>
       <c r="AF10">
-        <v>1.528044269075771</v>
+        <v>1.334225481724362</v>
       </c>
     </row>
     <row r="11" spans="1:32">
@@ -1398,94 +1398,94 @@
         <v>0.2973999644478771</v>
       </c>
       <c r="C11">
-        <v>0.2960223741642077</v>
+        <v>0.2960223741642074</v>
       </c>
       <c r="D11">
-        <v>0.2946922087454436</v>
+        <v>0.2947195743955275</v>
       </c>
       <c r="E11">
-        <v>0.2934076593169915</v>
+        <v>0.2934872257940609</v>
       </c>
       <c r="F11">
-        <v>0.292166996446796</v>
+        <v>0.292321267900254</v>
       </c>
       <c r="G11">
-        <v>0.2909685660560359</v>
+        <v>0.2912178986543565</v>
       </c>
       <c r="H11">
-        <v>0.2898107855738482</v>
+        <v>0.290173555645838</v>
       </c>
       <c r="I11">
-        <v>0.2886921403196173</v>
+        <v>0.2891848989328489</v>
       </c>
       <c r="J11">
-        <v>0.2876111800975953</v>
+        <v>0.2882487952819425</v>
       </c>
       <c r="K11">
-        <v>0.2865665159897468</v>
+        <v>0.2873623036941774</v>
       </c>
       <c r="L11">
-        <v>0.2855568173337468</v>
+        <v>0.2865226620977779</v>
       </c>
       <c r="M11">
-        <v>0.2845808088740187</v>
+        <v>0.2857272750999781</v>
       </c>
       <c r="N11">
-        <v>0.283637268074572</v>
+        <v>0.2849737027017114</v>
       </c>
       <c r="O11">
-        <v>0.2827250225832121</v>
+        <v>0.2842596498886042</v>
       </c>
       <c r="P11">
-        <v>0.2818429478374382</v>
+        <v>0.2835829570204361</v>
       </c>
       <c r="Q11">
-        <v>0.2809899648030308</v>
+        <v>0.2829415909489784</v>
       </c>
       <c r="R11">
-        <v>0.2801650378369678</v>
+        <v>0.2823336368010255</v>
       </c>
       <c r="S11">
-        <v>0.2793671726668894</v>
+        <v>0.281757290369588</v>
       </c>
       <c r="T11">
-        <v>0.2785954144798763</v>
+        <v>0.2812108510617187</v>
       </c>
       <c r="U11">
-        <v>0.2778488461138007</v>
+        <v>0.2806927153563543</v>
       </c>
       <c r="V11">
-        <v>0.2771265863449759</v>
+        <v>0.2802013707299586</v>
       </c>
       <c r="W11">
-        <v>0.2764277882662552</v>
+        <v>0.2797353900116944</v>
       </c>
       <c r="X11">
-        <v>0.2757516377501251</v>
+        <v>0.2792934261333875</v>
       </c>
       <c r="Y11">
-        <v>0.2750973519917073</v>
+        <v>0.278874207242724</v>
       </c>
       <c r="Z11">
-        <v>0.2744641781269204</v>
+        <v>0.2784765321509744</v>
       </c>
       <c r="AA11">
-        <v>0.2738513919213689</v>
+        <v>0.27809926608911</v>
       </c>
       <c r="AB11">
-        <v>0.2732582965258161</v>
+        <v>0.2777413367484906</v>
       </c>
       <c r="AC11">
-        <v>0.2726842212943727</v>
+        <v>0.2774017305843886</v>
       </c>
       <c r="AD11">
-        <v>0.2721285206617794</v>
+        <v>0.2770794893625009</v>
       </c>
       <c r="AE11">
-        <v>0.2715905730763989</v>
+        <v>0.2767737069303002</v>
       </c>
       <c r="AF11">
-        <v>0.2710697799857482</v>
+        <v>0.27648352619662</v>
       </c>
     </row>
     <row r="12" spans="1:32">
@@ -1496,94 +1496,94 @@
         <v>0.2021337213914698</v>
       </c>
       <c r="C12">
-        <v>0.195397820029489</v>
+        <v>0.1953978200294889</v>
       </c>
       <c r="D12">
-        <v>0.1890785348751237</v>
+        <v>0.1892067428715919</v>
       </c>
       <c r="E12">
-        <v>0.1831441568462355</v>
+        <v>0.1835070104762585</v>
       </c>
       <c r="F12">
-        <v>0.1775658239099951</v>
+        <v>0.1782513830558797</v>
       </c>
       <c r="G12">
-        <v>0.1723172301348837</v>
+        <v>0.1733980239410673</v>
       </c>
       <c r="H12">
-        <v>0.1673743677780995</v>
+        <v>0.1689097883752032</v>
       </c>
       <c r="I12">
-        <v>0.1627152983081793</v>
+        <v>0.1647536170488116</v>
       </c>
       <c r="J12">
-        <v>0.1583199488123431</v>
+        <v>0.1609000174445362</v>
       </c>
       <c r="K12">
-        <v>0.154169930708892</v>
+        <v>0.1573226190270393</v>
       </c>
       <c r="L12">
-        <v>0.1502483780889559</v>
+        <v>0.1539977907193739</v>
       </c>
       <c r="M12">
-        <v>0.1465398033590891</v>
+        <v>0.150904311069413</v>
       </c>
       <c r="N12">
-        <v>0.1430299681551352</v>
+        <v>0.1480230831143894</v>
       </c>
       <c r="O12">
-        <v>0.139705767755564</v>
+        <v>0.1453368872679133</v>
       </c>
       <c r="P12">
-        <v>0.136555127445149</v>
+        <v>0.1428301666371257</v>
       </c>
       <c r="Q12">
-        <v>0.1335669094725004</v>
+        <v>0.1404888400718982</v>
       </c>
       <c r="R12">
-        <v>0.1307308294118967</v>
+        <v>0.1383001389883871</v>
       </c>
       <c r="S12">
-        <v>0.1280373808847328</v>
+        <v>0.1362524646240347</v>
       </c>
       <c r="T12">
-        <v>0.125477767721826</v>
+        <v>0.1343352628930455</v>
       </c>
       <c r="U12">
-        <v>0.1230438427574323</v>
+        <v>0.1325389144388116</v>
       </c>
       <c r="V12">
-        <v>0.1207280525413818</v>
+        <v>0.1308546378376404</v>
       </c>
       <c r="W12">
-        <v>0.1185233873391641</v>
+        <v>0.1292744042085348</v>
       </c>
       <c r="X12">
-        <v>0.1164233358627249</v>
+        <v>0.1277908617365757</v>
       </c>
       <c r="Y12">
-        <v>0.1144218442385841</v>
+        <v>0.1263972688307302</v>
       </c>
       <c r="Z12">
-        <v>0.1125132787758591</v>
+        <v>0.1250874348172616</v>
       </c>
       <c r="AA12">
-        <v>0.1106923921459122</v>
+        <v>0.1238556672228029</v>
       </c>
       <c r="AB12">
-        <v>0.1089542926285317</v>
+        <v>0.1226967248310473</v>
       </c>
       <c r="AC12">
-        <v>0.1072944161175704</v>
+        <v>0.1216057758076144</v>
       </c>
       <c r="AD12">
-        <v>0.1057085006124628</v>
+        <v>0.1205783602820439</v>
       </c>
       <c r="AE12">
-        <v>0.1041925629516042</v>
+        <v>0.1196103568565926</v>
       </c>
       <c r="AF12">
-        <v>0.1027428775696872</v>
+        <v>0.1186979525806921</v>
       </c>
     </row>
     <row r="13" spans="1:32">
@@ -1591,97 +1591,97 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0.4269937661984928</v>
+        <v>0.4269937661984926</v>
       </c>
       <c r="C13">
-        <v>0.3582738118342019</v>
+        <v>0.3582738118342018</v>
       </c>
       <c r="D13">
-        <v>0.3022002283891198</v>
+        <v>0.3032626443992403</v>
       </c>
       <c r="E13">
-        <v>0.2562076661096697</v>
+        <v>0.2588466675780719</v>
       </c>
       <c r="F13">
-        <v>0.2182933634393182</v>
+        <v>0.2226922256387905</v>
       </c>
       <c r="G13">
-        <v>0.1868854507047761</v>
+        <v>0.1930342663720432</v>
       </c>
       <c r="H13">
-        <v>0.1607438637974714</v>
+        <v>0.1685261484434908</v>
       </c>
       <c r="I13">
-        <v>0.1388853849536362</v>
+        <v>0.1481318808133125</v>
       </c>
       <c r="J13">
-        <v>0.1205266335154097</v>
+        <v>0.1310480963613395</v>
       </c>
       <c r="K13">
-        <v>0.1050404832781257</v>
+        <v>0.1166470573311158</v>
       </c>
       <c r="L13">
-        <v>0.091922575852042</v>
+        <v>0.1044346713449581</v>
       </c>
       <c r="M13">
-        <v>0.08076546462767477</v>
+        <v>0.09401931345842945</v>
       </c>
       <c r="N13">
-        <v>0.07123855484217384</v>
+        <v>0.08508849227710041</v>
       </c>
       <c r="O13">
-        <v>0.06307246776017708</v>
+        <v>0.07739125569964599</v>
       </c>
       <c r="P13">
-        <v>0.05604679780085219</v>
+        <v>0.0707248288362259</v>
       </c>
       <c r="Q13">
-        <v>0.04998048384933336</v>
+        <v>0.06492439573848664</v>
       </c>
       <c r="R13">
-        <v>0.04472420383907806</v>
+        <v>0.05985523316232606</v>
       </c>
       <c r="S13">
-        <v>0.04015434216447802</v>
+        <v>0.05540661611470158</v>
       </c>
       <c r="T13">
-        <v>0.03616818502034757</v>
+        <v>0.05148706694017651</v>
       </c>
       <c r="U13">
-        <v>0.03268007841757056</v>
+        <v>0.04802062972690727</v>
       </c>
       <c r="V13">
-        <v>0.02961834400912202</v>
+        <v>0.0449439320087109</v>
       </c>
       <c r="W13">
-        <v>0.02692279383820602</v>
+        <v>0.04220385459216904</v>
       </c>
       <c r="X13">
-        <v>0.02454272027687677</v>
+        <v>0.0397556738093362</v>
       </c>
       <c r="Y13">
-        <v>0.02243526441771702</v>
+        <v>0.0375615728105274</v>
       </c>
       <c r="Z13">
-        <v>0.02056408699220685</v>
+        <v>0.03558944267872737</v>
       </c>
       <c r="AA13">
-        <v>0.01889828199726492</v>
+        <v>0.03381191232835034</v>
       </c>
       <c r="AB13">
-        <v>0.01741148572732626</v>
+        <v>0.03220555990735957</v>
       </c>
       <c r="AC13">
-        <v>0.01608114367106896</v>
+        <v>0.03075026888774875</v>
       </c>
       <c r="AD13">
-        <v>0.01488790537376062</v>
+        <v>0.02942870003480543</v>
       </c>
       <c r="AE13">
-        <v>0.01381512337017837</v>
+        <v>0.02822585660072241</v>
       </c>
       <c r="AF13">
-        <v>0.012848437026899</v>
+        <v>0.02712872484446409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>